<commit_message>
add final sesmo files and R version updates
</commit_message>
<xml_diff>
--- a/data/claves_estados_delegaciones_CVEGEO.xlsx
+++ b/data/claves_estados_delegaciones_CVEGEO.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abaezaca\Documents\MEGADAPT\SHV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abaezaca\Dropbox (ASU)\MEGADAPT\SHV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18135" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,105 +24,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Iztapalapa</t>
+  </si>
+  <si>
+    <t>Gustavo A. Madero</t>
+  </si>
+  <si>
+    <t>Álvaro Obregón</t>
+  </si>
+  <si>
+    <t>Tlalpan</t>
+  </si>
+  <si>
+    <t>Coyoacán</t>
+  </si>
+  <si>
+    <t>Cuauhtémoc</t>
+  </si>
+  <si>
+    <t>Venustiano Carranza</t>
+  </si>
+  <si>
+    <t>Benito Juárez</t>
+  </si>
+  <si>
+    <t>Xochimilco</t>
+  </si>
   <si>
     <t>Azcapotzalco</t>
   </si>
   <si>
-    <t>Coyoacán</t>
-  </si>
-  <si>
-    <t>Cuajimalpa</t>
-  </si>
-  <si>
-    <t>Cuauhtémoc</t>
-  </si>
-  <si>
     <t>Iztacalco</t>
   </si>
   <si>
-    <t>Iztapalapa</t>
+    <t>Miguel Hidalgo</t>
   </si>
   <si>
     <t>Tláhuac</t>
   </si>
   <si>
-    <t>Tlalpan</t>
-  </si>
-  <si>
-    <t>Xochimilco</t>
-  </si>
-  <si>
-    <t>Gustavo A. Madero</t>
-  </si>
-  <si>
-    <t>Benito Juárez</t>
-  </si>
-  <si>
-    <t>Álvaro Obregón</t>
-  </si>
-  <si>
-    <t>Magdalena Contreras</t>
-  </si>
-  <si>
-    <t>Miguel Hidalgo</t>
+    <t>La Magdalena Contreras</t>
+  </si>
+  <si>
+    <t>Cuajimalpa de Morelos</t>
   </si>
   <si>
     <t>Milpa Alta</t>
   </si>
   <si>
-    <t>Venustiano Carranza</t>
-  </si>
-  <si>
-    <t>delegacion</t>
-  </si>
-  <si>
-    <t>CVEGEO</t>
-  </si>
-  <si>
-    <t>estado de Mexico</t>
-  </si>
-  <si>
-    <t>clave AGEE</t>
-  </si>
-  <si>
-    <t>"15"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ciudad de mexico </t>
-  </si>
-  <si>
-    <t>"09"</t>
-  </si>
-  <si>
-    <t>hidalgo</t>
-  </si>
-  <si>
-    <t>Tlaxcala </t>
-  </si>
-  <si>
-    <t>Puebla</t>
-  </si>
-  <si>
-    <t>DOTACIÓN DE AGUA POTABLE L/HAB/D [2007]</t>
+    <t>Delegation</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>crecimiento_poblacional</t>
+  </si>
+  <si>
+    <t>DOTACION_AGUA_POTABLE_L_HAB_DIA_y2007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -145,16 +116,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -216,9 +184,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -251,9 +219,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -433,163 +401,236 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:D29"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>9002</v>
+      </c>
+      <c r="C2">
+        <v>-0.7</v>
+      </c>
+      <c r="D2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>9003</v>
+      </c>
+      <c r="C3">
+        <v>-0.3</v>
+      </c>
+      <c r="D3">
+        <v>312</v>
+      </c>
+    </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>9004</v>
+      </c>
+      <c r="C4">
+        <v>1.4</v>
+      </c>
+      <c r="D4">
+        <v>525</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>9010</v>
+        <v>9005</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>-0.1</v>
       </c>
       <c r="D5">
-        <v>391</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>9002</v>
+        <v>9006</v>
+      </c>
+      <c r="C6">
+        <v>0.4</v>
       </c>
       <c r="D6">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>9014</v>
+        <v>9007</v>
+      </c>
+      <c r="C7">
+        <v>0.4</v>
       </c>
       <c r="D7">
-        <v>455</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <v>9003</v>
+        <v>9008</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
       </c>
       <c r="D8">
-        <v>312</v>
+        <v>414</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>9004</v>
+        <v>9009</v>
+      </c>
+      <c r="C9">
+        <v>1.2</v>
       </c>
       <c r="D9">
-        <v>525</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>9015</v>
+        <v>9010</v>
+      </c>
+      <c r="C10">
+        <v>0.7</v>
       </c>
       <c r="D10">
-        <v>480</v>
+        <v>391</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>9005</v>
+        <v>9011</v>
+      </c>
+      <c r="C11">
+        <v>0.1</v>
       </c>
       <c r="D11">
-        <v>343</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>9006</v>
+        <v>9012</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>317</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>9007</v>
+        <v>9013</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
       </c>
       <c r="D13">
-        <v>238</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>9008</v>
+        <v>9014</v>
+      </c>
+      <c r="C14">
+        <v>1.8</v>
       </c>
       <c r="D14">
-        <v>414</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>9016</v>
+        <v>9015</v>
+      </c>
+      <c r="C15">
+        <v>0.2</v>
       </c>
       <c r="D15">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16">
-        <v>9009</v>
+        <v>9016</v>
+      </c>
+      <c r="C16">
+        <v>-0.4</v>
       </c>
       <c r="D16">
-        <v>231</v>
+        <v>478</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -597,86 +638,19 @@
         <v>6</v>
       </c>
       <c r="B17">
-        <v>9011</v>
+        <v>9017</v>
+      </c>
+      <c r="C17">
+        <v>-0.2</v>
       </c>
       <c r="D17">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18">
-        <v>9012</v>
-      </c>
-      <c r="D18">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19">
-        <v>9017</v>
-      </c>
-      <c r="D19">
         <v>337</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20">
-        <v>9013</v>
-      </c>
-      <c r="D20">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A28" r:id="rId1" tooltip="Tlaxcala" display="https://es.wikipedia.org/wiki/Tlaxcala"/>
-  </hyperlinks>
+  <sortState ref="A2:D17">
+    <sortCondition ref="B2:B17"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>